<commit_message>
iSDAsoil script almost ready
</commit_message>
<xml_diff>
--- a/data/soils_metadata.xlsx
+++ b/data/soils_metadata.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ToBackup\CGIAR_climate_action\datalake\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A384536-F43E-47C4-8697-D7FE5DAF16E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9CC00C6-E8E4-498C-A565-2B86F60746B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{F2056740-2197-4FB2-AFCE-FE2E99574F54}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
     <sheet name="iSDAsoil" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="stp" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="113">
   <si>
     <t>iSDAsoil</t>
   </si>
@@ -259,16 +259,124 @@
     <t>https://www.isda-africa.com/isdasoil/</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Ok</t>
-  </si>
-  <si>
-    <t>Running</t>
-  </si>
-  <si>
-    <t>To download</t>
+    <t>url</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>var_name</t>
+  </si>
+  <si>
+    <t>aluminium_extractable</t>
+  </si>
+  <si>
+    <t>bedrock_depth</t>
+  </si>
+  <si>
+    <t>bulk_density</t>
+  </si>
+  <si>
+    <t>calcium_extractable</t>
+  </si>
+  <si>
+    <t>carbon_organic</t>
+  </si>
+  <si>
+    <t>carbon_total</t>
+  </si>
+  <si>
+    <t>cation_exchange_capacity</t>
+  </si>
+  <si>
+    <t>clay_content</t>
+  </si>
+  <si>
+    <t>fcc</t>
+  </si>
+  <si>
+    <t>iron_extractable</t>
+  </si>
+  <si>
+    <t>magnesium_extractable</t>
+  </si>
+  <si>
+    <t>nitrogen_total</t>
+  </si>
+  <si>
+    <t>ph</t>
+  </si>
+  <si>
+    <t>phosphorous_extractable</t>
+  </si>
+  <si>
+    <t>potassium_extractable</t>
+  </si>
+  <si>
+    <t>sand_content</t>
+  </si>
+  <si>
+    <t>silt_content</t>
+  </si>
+  <si>
+    <t>stone_content</t>
+  </si>
+  <si>
+    <t>sulphur_extractable</t>
+  </si>
+  <si>
+    <t>texture_class</t>
+  </si>
+  <si>
+    <t>zinc_extractable</t>
+  </si>
+  <si>
+    <t>long_name</t>
+  </si>
+  <si>
+    <t>var_depth</t>
+  </si>
+  <si>
+    <t>var_stats</t>
+  </si>
+  <si>
+    <t>var_units</t>
+  </si>
+  <si>
+    <t>00-20cm</t>
+  </si>
+  <si>
+    <t>var_band</t>
+  </si>
+  <si>
+    <t>20-50cm</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>sd</t>
+  </si>
+  <si>
+    <t>ppm</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>g/cc</t>
+  </si>
+  <si>
+    <t>00-200cm</t>
+  </si>
+  <si>
+    <t>g/kg</t>
+  </si>
+  <si>
+    <t>cmol(+)/kg</t>
+  </si>
+  <si>
+    <t>%</t>
   </si>
 </sst>
 </file>
@@ -728,10 +836,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95987DEF-40CA-422E-8DC2-373AEAFDA16D}">
-  <dimension ref="A1:D80"/>
+  <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1476,14 +1584,35 @@
       </c>
       <c r="D80" s="4"/>
     </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A84" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="D2:D5"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="D8:D11"/>
-    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="D74:D75"/>
+    <mergeCell ref="A74:A76"/>
+    <mergeCell ref="D77:D80"/>
+    <mergeCell ref="A77:A80"/>
+    <mergeCell ref="D62:D65"/>
+    <mergeCell ref="A62:A65"/>
+    <mergeCell ref="D66:D69"/>
+    <mergeCell ref="A66:A69"/>
+    <mergeCell ref="D70:D73"/>
+    <mergeCell ref="A70:A73"/>
+    <mergeCell ref="D50:D53"/>
+    <mergeCell ref="A50:A53"/>
+    <mergeCell ref="D54:D57"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="D58:D61"/>
+    <mergeCell ref="A58:A61"/>
+    <mergeCell ref="D38:D41"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="D42:D45"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="D46:D49"/>
+    <mergeCell ref="A46:A49"/>
     <mergeCell ref="D34:D37"/>
     <mergeCell ref="A34:A37"/>
     <mergeCell ref="D12:D15"/>
@@ -1497,28 +1626,12 @@
     <mergeCell ref="D28:D31"/>
     <mergeCell ref="A28:A31"/>
     <mergeCell ref="A32:A33"/>
-    <mergeCell ref="D38:D41"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="D42:D45"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="D46:D49"/>
-    <mergeCell ref="A46:A49"/>
-    <mergeCell ref="D50:D53"/>
-    <mergeCell ref="A50:A53"/>
-    <mergeCell ref="D54:D57"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="D58:D61"/>
-    <mergeCell ref="A58:A61"/>
-    <mergeCell ref="D74:D75"/>
-    <mergeCell ref="A74:A76"/>
-    <mergeCell ref="D77:D80"/>
-    <mergeCell ref="A77:A80"/>
-    <mergeCell ref="D62:D65"/>
-    <mergeCell ref="A62:A65"/>
-    <mergeCell ref="D66:D69"/>
-    <mergeCell ref="A66:A69"/>
-    <mergeCell ref="D70:D73"/>
-    <mergeCell ref="A70:A73"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="A8:A11"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{F3B5C355-5176-446C-8CE7-BF6CD2A36002}"/>
@@ -1544,6 +1657,7 @@
     <hyperlink ref="D74" r:id="rId21" xr:uid="{EDCA5DFB-0C59-4CB7-AC10-9F8102D5915F}"/>
     <hyperlink ref="D76" r:id="rId22" xr:uid="{11555AB7-C52A-4D60-9326-E9C617A66381}"/>
     <hyperlink ref="D77" r:id="rId23" xr:uid="{3EEF1B99-F88B-4187-B475-D00DDE787407}"/>
+    <hyperlink ref="A84" r:id="rId24" xr:uid="{F283EB87-187E-4319-9F99-41E14D0ABB00}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1551,345 +1665,1073 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A00756B-5BA9-4F18-B2BF-1CD1A2A66434}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="85.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="85.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>8</v>
+        <v>75</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>67</v>
+        <v>102</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>10</v>
+        <v>98</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="F2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>106</v>
+      </c>
+      <c r="G3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>106</v>
+      </c>
+      <c r="G5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>109</v>
+      </c>
+      <c r="D6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E6" t="s">
         <v>17</v>
       </c>
-      <c r="B3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="F6" t="s">
+        <v>107</v>
+      </c>
+      <c r="G6" t="s">
+        <v>68</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" t="s">
+        <v>105</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>107</v>
+      </c>
+      <c r="G7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D8" t="s">
+        <v>104</v>
+      </c>
+      <c r="E8" t="s">
         <v>22</v>
       </c>
-      <c r="B4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="F8" t="s">
+        <v>108</v>
+      </c>
+      <c r="G8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" t="s">
+        <v>104</v>
+      </c>
+      <c r="E9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" t="s">
+        <v>108</v>
+      </c>
+      <c r="G9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" t="s">
+        <v>105</v>
+      </c>
+      <c r="E10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" t="s">
+        <v>108</v>
+      </c>
+      <c r="G10" t="s">
+        <v>68</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" t="s">
+        <v>108</v>
+      </c>
+      <c r="G11" t="s">
+        <v>68</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>101</v>
+      </c>
+      <c r="D12" t="s">
+        <v>104</v>
+      </c>
+      <c r="E12" t="s">
         <v>23</v>
       </c>
-      <c r="B5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="F12" t="s">
+        <v>106</v>
+      </c>
+      <c r="G12" t="s">
+        <v>68</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>103</v>
+      </c>
+      <c r="D13" t="s">
+        <v>104</v>
+      </c>
+      <c r="E13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" t="s">
+        <v>106</v>
+      </c>
+      <c r="G13" t="s">
+        <v>68</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D14" t="s">
+        <v>105</v>
+      </c>
+      <c r="E14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" t="s">
+        <v>106</v>
+      </c>
+      <c r="G14" t="s">
+        <v>68</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>103</v>
+      </c>
+      <c r="D15" t="s">
+        <v>105</v>
+      </c>
+      <c r="E15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" t="s">
+        <v>106</v>
+      </c>
+      <c r="G15" t="s">
+        <v>68</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>101</v>
+      </c>
+      <c r="D16" t="s">
+        <v>104</v>
+      </c>
+      <c r="E16" t="s">
         <v>25</v>
       </c>
-      <c r="B6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="F16" t="s">
+        <v>110</v>
+      </c>
+      <c r="G16" t="s">
+        <v>68</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>103</v>
+      </c>
+      <c r="D17" t="s">
+        <v>104</v>
+      </c>
+      <c r="E17" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" t="s">
+        <v>110</v>
+      </c>
+      <c r="G17" t="s">
+        <v>68</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>101</v>
+      </c>
+      <c r="D18" t="s">
+        <v>105</v>
+      </c>
+      <c r="E18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" t="s">
+        <v>110</v>
+      </c>
+      <c r="G18" t="s">
+        <v>68</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
+        <v>103</v>
+      </c>
+      <c r="D19" t="s">
+        <v>105</v>
+      </c>
+      <c r="E19" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" t="s">
+        <v>110</v>
+      </c>
+      <c r="G19" t="s">
+        <v>68</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>101</v>
+      </c>
+      <c r="D20" t="s">
+        <v>104</v>
+      </c>
+      <c r="E20" t="s">
         <v>27</v>
       </c>
-      <c r="B7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="F20" t="s">
+        <v>110</v>
+      </c>
+      <c r="G20" t="s">
+        <v>68</v>
+      </c>
+      <c r="H20" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>103</v>
+      </c>
+      <c r="D21" t="s">
+        <v>104</v>
+      </c>
+      <c r="E21" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" t="s">
+        <v>110</v>
+      </c>
+      <c r="G21" t="s">
+        <v>68</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>101</v>
+      </c>
+      <c r="D22" t="s">
+        <v>105</v>
+      </c>
+      <c r="E22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F22" t="s">
+        <v>110</v>
+      </c>
+      <c r="G22" t="s">
+        <v>68</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>81</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>103</v>
+      </c>
+      <c r="D23" t="s">
+        <v>105</v>
+      </c>
+      <c r="E23" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" t="s">
+        <v>110</v>
+      </c>
+      <c r="G23" t="s">
+        <v>68</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>101</v>
+      </c>
+      <c r="D24" t="s">
+        <v>104</v>
+      </c>
+      <c r="E24" t="s">
         <v>30</v>
       </c>
-      <c r="B8" t="s">
-        <v>68</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="F24" t="s">
+        <v>111</v>
+      </c>
+      <c r="G24" t="s">
+        <v>68</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>82</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25" t="s">
+        <v>103</v>
+      </c>
+      <c r="D25" t="s">
+        <v>104</v>
+      </c>
+      <c r="E25" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25" t="s">
+        <v>111</v>
+      </c>
+      <c r="G25" t="s">
+        <v>68</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>82</v>
+      </c>
+      <c r="B26">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s">
+        <v>101</v>
+      </c>
+      <c r="D26" t="s">
+        <v>105</v>
+      </c>
+      <c r="E26" t="s">
+        <v>30</v>
+      </c>
+      <c r="F26" t="s">
+        <v>111</v>
+      </c>
+      <c r="G26" t="s">
+        <v>68</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>82</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="C27" t="s">
+        <v>103</v>
+      </c>
+      <c r="D27" t="s">
+        <v>105</v>
+      </c>
+      <c r="E27" t="s">
+        <v>30</v>
+      </c>
+      <c r="F27" t="s">
+        <v>111</v>
+      </c>
+      <c r="G27" t="s">
+        <v>68</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>83</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>101</v>
+      </c>
+      <c r="D28" t="s">
+        <v>104</v>
+      </c>
+      <c r="E28" t="s">
         <v>31</v>
       </c>
-      <c r="B9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="F28" t="s">
+        <v>112</v>
+      </c>
+      <c r="G28" t="s">
+        <v>68</v>
+      </c>
+      <c r="H28" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29" t="s">
+        <v>103</v>
+      </c>
+      <c r="D29" t="s">
+        <v>104</v>
+      </c>
+      <c r="E29" t="s">
+        <v>31</v>
+      </c>
+      <c r="F29" t="s">
+        <v>112</v>
+      </c>
+      <c r="G29" t="s">
+        <v>68</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>83</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30" t="s">
+        <v>101</v>
+      </c>
+      <c r="D30" t="s">
+        <v>105</v>
+      </c>
+      <c r="E30" t="s">
+        <v>31</v>
+      </c>
+      <c r="F30" t="s">
+        <v>112</v>
+      </c>
+      <c r="G30" t="s">
+        <v>68</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>83</v>
+      </c>
+      <c r="B31">
+        <v>4</v>
+      </c>
+      <c r="C31" t="s">
+        <v>103</v>
+      </c>
+      <c r="D31" t="s">
+        <v>105</v>
+      </c>
+      <c r="E31" t="s">
+        <v>31</v>
+      </c>
+      <c r="F31" t="s">
+        <v>112</v>
+      </c>
+      <c r="G31" t="s">
+        <v>68</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>84</v>
+      </c>
+      <c r="E32" t="s">
         <v>33</v>
       </c>
-      <c r="B10" t="s">
+      <c r="G32" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="H32" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D10" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>84</v>
+      </c>
+      <c r="E33" t="s">
         <v>71</v>
       </c>
-      <c r="B11" t="s">
+      <c r="G33" t="s">
         <v>69</v>
       </c>
-      <c r="C11" t="s">
+      <c r="H33" t="s">
         <v>36</v>
       </c>
-      <c r="D11" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>85</v>
+      </c>
+      <c r="E34" t="s">
         <v>38</v>
       </c>
-      <c r="B12" t="s">
-        <v>68</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="G34" t="s">
+        <v>68</v>
+      </c>
+      <c r="H34" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>86</v>
+      </c>
+      <c r="E35" t="s">
         <v>40</v>
       </c>
-      <c r="B13" t="s">
-        <v>68</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="G35" t="s">
+        <v>68</v>
+      </c>
+      <c r="H35" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D13" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>87</v>
+      </c>
+      <c r="E36" t="s">
         <v>42</v>
       </c>
-      <c r="B14" t="s">
-        <v>68</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="G36" t="s">
+        <v>68</v>
+      </c>
+      <c r="H36" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>88</v>
+      </c>
+      <c r="E37" t="s">
         <v>44</v>
       </c>
-      <c r="B15" t="s">
-        <v>68</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="G37" t="s">
+        <v>68</v>
+      </c>
+      <c r="H37" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D15" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>89</v>
+      </c>
+      <c r="E38" t="s">
         <v>46</v>
       </c>
-      <c r="B16" t="s">
-        <v>68</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="G38" t="s">
+        <v>68</v>
+      </c>
+      <c r="H38" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>90</v>
+      </c>
+      <c r="E39" t="s">
         <v>48</v>
       </c>
-      <c r="B17" t="s">
-        <v>68</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="G39" t="s">
+        <v>68</v>
+      </c>
+      <c r="H39" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>91</v>
+      </c>
+      <c r="E40" t="s">
         <v>50</v>
       </c>
-      <c r="B18" t="s">
-        <v>68</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="G40" t="s">
+        <v>68</v>
+      </c>
+      <c r="H40" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>92</v>
+      </c>
+      <c r="E41" t="s">
         <v>52</v>
       </c>
-      <c r="B19" t="s">
-        <v>68</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="G41" t="s">
+        <v>68</v>
+      </c>
+      <c r="H41" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>93</v>
+      </c>
+      <c r="E42" t="s">
         <v>54</v>
       </c>
-      <c r="B20" t="s">
-        <v>68</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="G42" t="s">
+        <v>68</v>
+      </c>
+      <c r="H42" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>94</v>
+      </c>
+      <c r="E43" t="s">
         <v>56</v>
       </c>
-      <c r="B21" t="s">
-        <v>68</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="G43" t="s">
+        <v>68</v>
+      </c>
+      <c r="H43" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>95</v>
+      </c>
+      <c r="E44" t="s">
         <v>58</v>
       </c>
-      <c r="B22" t="s">
+      <c r="G44" t="s">
         <v>69</v>
       </c>
-      <c r="C22" t="s">
+      <c r="H44" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>95</v>
+      </c>
+      <c r="E45" t="s">
         <v>70</v>
       </c>
-      <c r="B23" t="s">
+      <c r="G45" t="s">
         <v>69</v>
       </c>
-      <c r="C23" t="s">
+      <c r="H45" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>96</v>
+      </c>
+      <c r="E46" t="s">
         <v>62</v>
       </c>
-      <c r="B24" t="s">
-        <v>68</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="G46" t="s">
+        <v>68</v>
+      </c>
+      <c r="H46" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C15" r:id="rId1" xr:uid="{3E911314-C50B-4F2A-BB8E-0F8377AD47D8}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{7B9B9D79-D64A-4F76-BE74-B2B78E6D2E9B}"/>
-    <hyperlink ref="C3" r:id="rId3" xr:uid="{75896B35-5BAB-4931-A5FF-B0AB7B99C6AE}"/>
-    <hyperlink ref="C4" r:id="rId4" xr:uid="{13CA615A-33C8-4B0E-84AE-0255BD0161A5}"/>
-    <hyperlink ref="C5" r:id="rId5" xr:uid="{F1D1D4A5-D46E-4993-9156-E307094A0602}"/>
-    <hyperlink ref="C6" r:id="rId6" xr:uid="{CC7AEE29-B161-445F-B966-BEC7B39C411D}"/>
-    <hyperlink ref="C7" r:id="rId7" xr:uid="{2A11D17B-A402-4B05-9202-997741E37F5E}"/>
-    <hyperlink ref="C8" r:id="rId8" xr:uid="{6E3A7A9E-0F97-41DF-866A-0C3C8AC165F3}"/>
-    <hyperlink ref="C9" r:id="rId9" xr:uid="{35854FE2-C1C9-4ABD-83BF-F48CCB8010A7}"/>
-    <hyperlink ref="A26" r:id="rId10" xr:uid="{F283EB87-187E-4319-9F99-41E14D0ABB00}"/>
-    <hyperlink ref="C10" r:id="rId11" xr:uid="{1A311D67-F301-4A44-ACC0-C7E7DFA515C5}"/>
-    <hyperlink ref="C12" r:id="rId12" xr:uid="{8E564EE1-86C0-47A0-AA4B-99734FE8D287}"/>
-    <hyperlink ref="C13" r:id="rId13" xr:uid="{24E06580-8115-4508-8739-38587903F9C0}"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{7B9B9D79-D64A-4F76-BE74-B2B78E6D2E9B}"/>
+    <hyperlink ref="H35" r:id="rId2" xr:uid="{24E06580-8115-4508-8739-38587903F9C0}"/>
+    <hyperlink ref="H34" r:id="rId3" xr:uid="{8E564EE1-86C0-47A0-AA4B-99734FE8D287}"/>
+    <hyperlink ref="H32" r:id="rId4" xr:uid="{1A311D67-F301-4A44-ACC0-C7E7DFA515C5}"/>
+    <hyperlink ref="H37" r:id="rId5" xr:uid="{3E911314-C50B-4F2A-BB8E-0F8377AD47D8}"/>
+    <hyperlink ref="H3:H5" r:id="rId6" display="https://isdasoil.s3.amazonaws.com/soil_data/aluminium_extractable/aluminium_extractable.tif" xr:uid="{9C8BD4A1-42A3-48E0-813B-2C19BD4D969B}"/>
+    <hyperlink ref="H6:H7" r:id="rId7" display="https://isdasoil.s3.amazonaws.com/soil_data/bulk_density/bulk_density.tif" xr:uid="{19381AE3-D482-48B1-ADE6-B565B92A8B5C}"/>
+    <hyperlink ref="H8" r:id="rId8" display="https://isdasoil.s3.amazonaws.com/soil_data/calcium_extractable/calcium_extractable.tif" xr:uid="{B7E9C1C6-DE79-4F8C-9F6E-C2E09EA17557}"/>
+    <hyperlink ref="H9" r:id="rId9" display="https://isdasoil.s3.amazonaws.com/soil_data/calcium_extractable/calcium_extractable.tif" xr:uid="{0BDB1C57-A51C-4C2A-AAFC-4AA6E9923CDF}"/>
+    <hyperlink ref="H10" r:id="rId10" display="https://isdasoil.s3.amazonaws.com/soil_data/calcium_extractable/calcium_extractable.tif" xr:uid="{F89A0AC3-038D-4381-9CB6-7E2A9373875C}"/>
+    <hyperlink ref="H11" r:id="rId11" display="https://isdasoil.s3.amazonaws.com/soil_data/calcium_extractable/calcium_extractable.tif" xr:uid="{6889CF3A-E315-485B-BF11-6FEE8F53E176}"/>
+    <hyperlink ref="H12" r:id="rId12" display="https://isdasoil.s3.amazonaws.com/soil_data/carbon_organic/carbon_organic.tif" xr:uid="{47142A10-FFBC-4C5B-A45E-CBDDB54AD42C}"/>
+    <hyperlink ref="H13" r:id="rId13" display="https://isdasoil.s3.amazonaws.com/soil_data/carbon_organic/carbon_organic.tif" xr:uid="{96A6B811-36A2-4A61-B666-9BF06FF7427B}"/>
+    <hyperlink ref="H14" r:id="rId14" display="https://isdasoil.s3.amazonaws.com/soil_data/carbon_organic/carbon_organic.tif" xr:uid="{DC6ABCE5-3104-4439-9697-F712FEC47D81}"/>
+    <hyperlink ref="H15" r:id="rId15" display="https://isdasoil.s3.amazonaws.com/soil_data/carbon_organic/carbon_organic.tif" xr:uid="{0E6D4286-C74A-4A8C-A2D5-101037195F71}"/>
+    <hyperlink ref="H16" r:id="rId16" display="https://isdasoil.s3.amazonaws.com/soil_data/magnesium_extractable/magnesium_extractable.tif" xr:uid="{D858BF68-099C-479A-9821-4F91A168ABB1}"/>
+    <hyperlink ref="H17" r:id="rId17" display="https://isdasoil.s3.amazonaws.com/soil_data/magnesium_extractable/magnesium_extractable.tif" xr:uid="{5946A20E-3980-417B-BD1A-0FF6C3D3F9F3}"/>
+    <hyperlink ref="H18" r:id="rId18" display="https://isdasoil.s3.amazonaws.com/soil_data/magnesium_extractable/magnesium_extractable.tif" xr:uid="{7010BD57-7581-443E-AB2E-5F4F6BAF1AFB}"/>
+    <hyperlink ref="H19" r:id="rId19" display="https://isdasoil.s3.amazonaws.com/soil_data/magnesium_extractable/magnesium_extractable.tif" xr:uid="{9551D032-13BB-4065-A9E7-ABE7B2190B28}"/>
+    <hyperlink ref="H20" r:id="rId20" display="https://isdasoil.s3.amazonaws.com/soil_data/ph/ph.tif" xr:uid="{F6F9361E-5EAD-4B16-9969-631C83895051}"/>
+    <hyperlink ref="H21" r:id="rId21" display="https://isdasoil.s3.amazonaws.com/soil_data/ph/ph.tif" xr:uid="{F2B34E0B-ABAC-4170-A0AF-FD2186C70294}"/>
+    <hyperlink ref="H22" r:id="rId22" display="https://isdasoil.s3.amazonaws.com/soil_data/ph/ph.tif" xr:uid="{0DED9D91-38AB-44AE-AB97-D1B5C4842985}"/>
+    <hyperlink ref="H23" r:id="rId23" display="https://isdasoil.s3.amazonaws.com/soil_data/ph/ph.tif" xr:uid="{9F79B226-DA12-48BD-B59C-C344EE2897D6}"/>
+    <hyperlink ref="H24" r:id="rId24" display="https://isdasoil.s3.amazonaws.com/soil_data/ph/ph.tif" xr:uid="{93695154-14DF-49B1-B62F-3FA5E374ACD2}"/>
+    <hyperlink ref="H25" r:id="rId25" display="https://isdasoil.s3.amazonaws.com/soil_data/ph/ph.tif" xr:uid="{913B7E1F-4E17-48B2-9857-8AE728FEFBCE}"/>
+    <hyperlink ref="H26" r:id="rId26" display="https://isdasoil.s3.amazonaws.com/soil_data/ph/ph.tif" xr:uid="{F90C1D7F-74C7-4095-B0FF-6D40BAD6C1CB}"/>
+    <hyperlink ref="H27" r:id="rId27" display="https://isdasoil.s3.amazonaws.com/soil_data/ph/ph.tif" xr:uid="{9FF21F88-D55A-4B42-B966-E081AF53A8B8}"/>
+    <hyperlink ref="H28" r:id="rId28" display="https://isdasoil.s3.amazonaws.com/soil_data/ph/ph.tif" xr:uid="{5AE60FD3-833D-4A09-A157-10793C071A7C}"/>
+    <hyperlink ref="H29" r:id="rId29" display="https://isdasoil.s3.amazonaws.com/soil_data/ph/ph.tif" xr:uid="{778EC22A-7482-497F-A299-B4235924E33F}"/>
+    <hyperlink ref="H30" r:id="rId30" display="https://isdasoil.s3.amazonaws.com/soil_data/ph/ph.tif" xr:uid="{84238767-AC37-4DD9-B105-0E96DEFC7896}"/>
+    <hyperlink ref="H31" r:id="rId31" display="https://isdasoil.s3.amazonaws.com/soil_data/ph/ph.tif" xr:uid="{1C3C86F2-B973-4909-8FA1-936D1C91F211}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>